<commit_message>
#19 #21 #27 #28 #29 #30 #31 #32 #33 #34 #36 #39 #40 #42 #44 #47 #48 #49 #50 #51 #52 #54 #57
</commit_message>
<xml_diff>
--- a/documentation/charts.xlsx
+++ b/documentation/charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WORLD TEMP" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>ОБЛАЧНОСТЬ</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>GRADE 5</t>
+  </si>
+  <si>
+    <t>CHAOS</t>
+  </si>
+  <si>
+    <t>GM6</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +203,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,15 +1418,15 @@
       </c>
       <c r="C3" s="3">
         <f ca="1">RAND()</f>
-        <v>0.77851250920129456</v>
+        <v>0.98624812030642151</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">MAX((C3-0.4)*20,0)</f>
-        <v>7.5702501840258911</v>
+        <v>11.72496240612843</v>
       </c>
       <c r="F3" s="3">
         <f ca="1">E3/12</f>
-        <v>0.63085418200215759</v>
+        <v>0.97708020051070255</v>
       </c>
       <c r="G3" s="3">
         <f>ABS(14-B3)/13</f>
@@ -1437,15 +1444,15 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C26" ca="1" si="0">RAND()</f>
-        <v>0.51813694888550299</v>
+        <v>0.73190800734903994</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E26" ca="1" si="1">MAX((C4-0.4)*20,0)</f>
-        <v>2.3627389777100594</v>
+        <v>6.6381601469807983</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F26" ca="1" si="2">E4/12</f>
-        <v>0.19689491480917162</v>
+        <v>0.55318001224839985</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ref="G4:G26" si="3">ABS(14-B4)/13</f>
@@ -1463,15 +1470,15 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31031510666808881</v>
+        <v>0.44532764062739738</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>0.90655281254794717</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>7.5546067712328926E-2</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="3"/>
@@ -1489,15 +1496,15 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96130919887188426</v>
+        <v>0.49092105539129727</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11.226183977437685</v>
+        <v>1.8184211078259449</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93551533145314048</v>
+        <v>0.15153509231882875</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="3"/>
@@ -1505,7 +1512,7 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.93551533145314048</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1515,7 +1522,7 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26444917772965226</v>
+        <v>0.39764354640012023</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1541,15 +1548,15 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24853447076311996</v>
+        <v>0.71286374052721457</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>6.257274810544291</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.52143956754535759</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="3"/>
@@ -1567,15 +1574,15 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44709211571249785</v>
+        <v>0.99612123931739815</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94184231424995657</v>
+        <v>11.922424786347962</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7.8486859520829719E-2</v>
+        <v>0.99353539886233022</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="3"/>
@@ -1583,7 +1590,7 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.53846153846153844</v>
+        <v>0.99353539886233022</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1593,15 +1600,15 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45718553006372853</v>
+        <v>3.5656121308690225E-2</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1437106012745701</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9.5309216772880845E-2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="3"/>
@@ -1619,15 +1626,15 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5012033232905545</v>
+        <v>0.94678960123989997</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0240664658110896</v>
+        <v>10.935792024797999</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16867220548425746</v>
+        <v>0.91131600206649999</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="3"/>
@@ -1635,7 +1642,7 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.38461538461538464</v>
+        <v>0.91131600206649999</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1645,15 +1652,15 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53592913148724775</v>
+        <v>0.78992616119742209</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7185826297449545</v>
+        <v>7.7985232239484414</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2265485524787462</v>
+        <v>0.64987693532903679</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="3"/>
@@ -1661,7 +1668,7 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.30769230769230771</v>
+        <v>0.64987693532903679</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1671,15 +1678,15 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5572395789187119</v>
+        <v>0.92944368915743214</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1447915783742375</v>
+        <v>10.588873783148642</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26206596486451977</v>
+        <v>0.8824061485957202</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="3"/>
@@ -1687,7 +1694,7 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.26206596486451977</v>
+        <v>0.8824061485957202</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1697,15 +1704,15 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68386267957567304</v>
+        <v>0.25912436305066844</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6772535915134608</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47310446595945504</v>
+        <v>0</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
@@ -1713,7 +1720,7 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.47310446595945504</v>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1723,15 +1730,15 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3593380972749052E-2</v>
+        <v>0.47767750292925826</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1.5535500585851647</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.12946250488209707</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="3"/>
@@ -1739,7 +1746,7 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>7.6923076923076927E-2</v>
+        <v>0.12946250488209707</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1749,15 +1756,15 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28792578025157778</v>
+        <v>0.5975849341622963</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3.9516986832459255</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.32930822360382711</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="3"/>
@@ -1765,7 +1772,7 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>0.32930822360382711</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1775,15 +1782,15 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81214760049281509</v>
+        <v>0.93859203325930185</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2429520098563014</v>
+        <v>10.771840665186037</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68691266748802515</v>
+        <v>0.89765338876550305</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="3"/>
@@ -1791,7 +1798,7 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.68691266748802515</v>
+        <v>0.89765338876550305</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1801,15 +1808,15 @@
       </c>
       <c r="C18" s="3">
         <f ca="1">RAND()</f>
-        <v>0.84317689119480266</v>
+        <v>0.91404288216693574</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8635378238960527</v>
+        <v>10.280857643338715</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.73862815199133769</v>
+        <v>0.85673813694489287</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="3"/>
@@ -1817,7 +1824,7 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.73862815199133769</v>
+        <v>0.85673813694489287</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1827,7 +1834,7 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21841622091976576</v>
+        <v>5.2794582632899267E-2</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1853,15 +1860,15 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.176726094766404E-2</v>
+        <v>0.58363458286779946</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3.6726916573559887</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.30605763811299908</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="3"/>
@@ -1879,15 +1886,15 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30188197801184258</v>
+        <v>0.99988398560989689</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>11.997679712197938</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.99980664268316144</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="3"/>
@@ -1895,7 +1902,7 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.38461538461538464</v>
+        <v>0.99980664268316144</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1905,15 +1912,15 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21925282335442142</v>
+        <v>0.41416866695562271</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>0.28337333911245377</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2.3614444926037814E-2</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="3"/>
@@ -1931,15 +1938,15 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45381509598490355</v>
+        <v>0.69483908363307267</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0763019196980705</v>
+        <v>5.8967816726614526</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8.9691826641505878E-2</v>
+        <v>0.49139847272178772</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="3"/>
@@ -1957,7 +1964,7 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12917918309962739</v>
+        <v>0.33553342581520373</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1983,15 +1990,15 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44545251355498161</v>
+        <v>0.70061592883415724</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90905027109963177</v>
+        <v>6.0123185766831444</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7.5754189258302643E-2</v>
+        <v>0.5010265480569287</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="3"/>
@@ -2009,15 +2016,15 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89061976331799708</v>
+        <v>3.9560207958790228E-2</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8123952663599407</v>
+        <v>0</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8176996055299951</v>
+        <v>0</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="3"/>
@@ -2025,7 +2032,7 @@
       </c>
       <c r="H26" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.8176996055299951</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2099,7 +2106,7 @@
         <v>0.24000000000000002</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:E12" si="2">0.2+(A4*0.03)</f>
+        <f t="shared" ref="D4:D12" si="2">0.2+(A4*0.03)</f>
         <v>0.26</v>
       </c>
       <c r="F4">
@@ -2651,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,15 +2669,21 @@
     <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2678,8 +2691,15 @@
         <f>POWER(B3 * 10,1.8)</f>
         <v>63.095734448019364</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="7">
+        <f>(1/(F3*0.2))*0.99*1000</f>
+        <v>12374.999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
@@ -2689,7 +2709,7 @@
         <v>219.71210866122351</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" ref="B5:B7" si="1">B4+1</f>
         <v>3</v>
@@ -2699,7 +2719,7 @@
         <v>455.84611570090664</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2709,7 +2729,7 @@
         <v>765.08199983202962</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2719,7 +2739,7 @@
         <v>1143.2626298183159</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -2736,8 +2756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,15 +2802,15 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F6" si="1">MOD((MOD(C3/150,1)*150)/50,1)*50/25</f>
+        <f>MOD((MOD(C3/150,1)*150)/50,1)*50/25</f>
         <v>6.4000000000000015E-2</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G6" si="2">(MOD(C3/150,1)*150)/50</f>
+        <f>(MOD(C3/150,1)*150)/50</f>
         <v>3.2000000000000008E-2</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H6" si="3">C3/150</f>
+        <f>C3/150</f>
         <v>1.0666666666666668E-2</v>
       </c>
     </row>
@@ -2807,15 +2827,15 @@
         <v>5.4</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="1"/>
+        <f>MOD((MOD(C4/150,1)*150)/50,1)*50/25</f>
         <v>0.21600000000000003</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" si="2"/>
+        <f>(MOD(C4/150,1)*150)/50</f>
         <v>0.10800000000000001</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="3"/>
+        <f>C4/150</f>
         <v>3.6000000000000004E-2</v>
       </c>
     </row>
@@ -2832,15 +2852,15 @@
         <v>12.800000000000002</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="1"/>
+        <f>MOD((MOD(C5/150,1)*150)/50,1)*50/25</f>
         <v>0.51200000000000012</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="2"/>
+        <f>(MOD(C5/150,1)*150)/50</f>
         <v>0.25600000000000006</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" si="3"/>
+        <f>C5/150</f>
         <v>8.5333333333333344E-2</v>
       </c>
     </row>
@@ -2857,15 +2877,15 @@
         <v>0</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="1"/>
+        <f>MOD((MOD(C6/150,1)*150)/50,1)*50/25</f>
         <v>1</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="2"/>
+        <f>(MOD(C6/150,1)*150)/50</f>
         <v>0.5</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="3"/>
+        <f>C6/150</f>
         <v>0.16666666666666666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#8 #21 #26 #29 #30 #45 #47 #49 #52 #62 #63
</commit_message>
<xml_diff>
--- a/documentation/charts.xlsx
+++ b/documentation/charts.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WORLD TEMP" sheetId="1" r:id="rId1"/>
     <sheet name="WEATHER" sheetId="5" r:id="rId2"/>
-    <sheet name="CHAOS LEVEL" sheetId="6" r:id="rId3"/>
-    <sheet name="PLAYER TEMP" sheetId="2" r:id="rId4"/>
-    <sheet name="MONEY" sheetId="3" r:id="rId5"/>
-    <sheet name="SPAWN POWERS" sheetId="4" r:id="rId6"/>
+    <sheet name="HUD" sheetId="7" r:id="rId3"/>
+    <sheet name="CHAOS LEVEL" sheetId="6" r:id="rId4"/>
+    <sheet name="PLAYER TEMP" sheetId="2" r:id="rId5"/>
+    <sheet name="MONEY" sheetId="3" r:id="rId6"/>
+    <sheet name="SPAWN POWERS" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>ОБЛАЧНОСТЬ</t>
   </si>
@@ -152,6 +153,12 @@
   </si>
   <si>
     <t>GM6</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>IMAGE</t>
   </si>
 </sst>
 </file>
@@ -486,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1390,7 @@
   <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,15 +1425,15 @@
       </c>
       <c r="C3" s="3">
         <f ca="1">RAND()</f>
-        <v>0.98624812030642151</v>
+        <v>0.70495548776819184</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">MAX((C3-0.4)*20,0)</f>
-        <v>11.72496240612843</v>
+        <v>6.0991097553638358</v>
       </c>
       <c r="F3" s="3">
         <f ca="1">E3/12</f>
-        <v>0.97708020051070255</v>
+        <v>0.50825914628031965</v>
       </c>
       <c r="G3" s="3">
         <f>ABS(14-B3)/13</f>
@@ -1444,15 +1451,15 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C26" ca="1" si="0">RAND()</f>
-        <v>0.73190800734903994</v>
+        <v>0.29920265833098536</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E26" ca="1" si="1">MAX((C4-0.4)*20,0)</f>
-        <v>6.6381601469807983</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ref="F4:F26" ca="1" si="2">E4/12</f>
-        <v>0.55318001224839985</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ref="G4:G26" si="3">ABS(14-B4)/13</f>
@@ -1470,15 +1477,15 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44532764062739738</v>
+        <v>9.7473401375907875E-2</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90655281254794717</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7.5546067712328926E-2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="3"/>
@@ -1496,15 +1503,15 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49092105539129727</v>
+        <v>0.97892311775729079</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8184211078259449</v>
+        <v>11.578462355145815</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.15153509231882875</v>
+        <v>0.96487186292881788</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="3"/>
@@ -1512,7 +1519,7 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.76923076923076927</v>
+        <v>0.96487186292881788</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1522,15 +1529,15 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39764354640012023</v>
+        <v>0.53602725968137954</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.7205451936275904</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.22671209946896587</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="3"/>
@@ -1548,15 +1555,15 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71286374052721457</v>
+        <v>0.9046661323971007</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.257274810544291</v>
+        <v>10.093322647942014</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.52143956754535759</v>
+        <v>0.8411102206618345</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="3"/>
@@ -1564,7 +1571,7 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61538461538461542</v>
+        <v>0.8411102206618345</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1574,15 +1581,15 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99612123931739815</v>
+        <v>0.86568084261055411</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11.922424786347962</v>
+        <v>9.3136168522110818</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.99353539886233022</v>
+        <v>0.77613473768425678</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="3"/>
@@ -1590,7 +1597,7 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99353539886233022</v>
+        <v>0.77613473768425678</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1600,15 +1607,15 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5656121308690225E-2</v>
+        <v>0.69099063117876469</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5.8198126235752934</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.48498438529794113</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="3"/>
@@ -1616,7 +1623,7 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.46153846153846156</v>
+        <v>0.48498438529794113</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1626,15 +1633,15 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94678960123989997</v>
+        <v>0.49735511489268458</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.935792024797999</v>
+        <v>1.9471022978536912</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.91131600206649999</v>
+        <v>0.16225852482114092</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="3"/>
@@ -1642,7 +1649,7 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.91131600206649999</v>
+        <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1652,15 +1659,15 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78992616119742209</v>
+        <v>0.86026390224790439</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7985232239484414</v>
+        <v>9.2052780449580869</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.64987693532903679</v>
+        <v>0.76710650374650724</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="3"/>
@@ -1668,7 +1675,7 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.64987693532903679</v>
+        <v>0.76710650374650724</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1678,15 +1685,15 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92944368915743214</v>
+        <v>0.68477968438556835</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.588873783148642</v>
+        <v>5.6955936877113666</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8824061485957202</v>
+        <v>0.47463280730928054</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="3"/>
@@ -1694,7 +1701,7 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.8824061485957202</v>
+        <v>0.47463280730928054</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1704,7 +1711,7 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25912436305066844</v>
+        <v>0.25031236403669199</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1730,15 +1737,15 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47767750292925826</v>
+        <v>0.16807731447506447</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5535500585851647</v>
+        <v>0</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12946250488209707</v>
+        <v>0</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="3"/>
@@ -1746,7 +1753,7 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.12946250488209707</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1756,15 +1763,15 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5975849341622963</v>
+        <v>0.52521571772110043</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9516986832459255</v>
+        <v>2.5043143544220081</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32930822360382711</v>
+        <v>0.20869286286850067</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="3"/>
@@ -1772,7 +1779,7 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.32930822360382711</v>
+        <v>0.20869286286850067</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1782,15 +1789,15 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93859203325930185</v>
+        <v>0.38874889248844335</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.771840665186037</v>
+        <v>0</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89765338876550305</v>
+        <v>0</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="3"/>
@@ -1798,7 +1805,7 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.89765338876550305</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1808,15 +1815,15 @@
       </c>
       <c r="C18" s="3">
         <f ca="1">RAND()</f>
-        <v>0.91404288216693574</v>
+        <v>0.51242450550358554</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.280857643338715</v>
+        <v>2.2484901100717103</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85673813694489287</v>
+        <v>0.18737417583930918</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="3"/>
@@ -1824,7 +1831,7 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.85673813694489287</v>
+        <v>0.18737417583930918</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1834,7 +1841,7 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2794582632899267E-2</v>
+        <v>0.15683169422185195</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1860,15 +1867,15 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58363458286779946</v>
+        <v>0.27567675512286371</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6726916573559887</v>
+        <v>0</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30605763811299908</v>
+        <v>0</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="3"/>
@@ -1886,15 +1893,15 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99988398560989689</v>
+        <v>0.5787651167845328</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11.997679712197938</v>
+        <v>3.5753023356906555</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.99980664268316144</v>
+        <v>0.29794186130755462</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="3"/>
@@ -1902,7 +1909,7 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99980664268316144</v>
+        <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1912,15 +1919,15 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41416866695562271</v>
+        <v>0.92410924680525419</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28337333911245377</v>
+        <v>10.482184936105083</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.3614444926037814E-2</v>
+        <v>0.87351541134209032</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="3"/>
@@ -1928,7 +1935,7 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.46153846153846156</v>
+        <v>0.87351541134209032</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1938,15 +1945,15 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69483908363307267</v>
+        <v>0.29303778344106191</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8967816726614526</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49139847272178772</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="3"/>
@@ -1964,15 +1971,15 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33553342581520373</v>
+        <v>0.86391598545991899</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>9.2783197091983798</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.77319330909986494</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="3"/>
@@ -1980,7 +1987,7 @@
       </c>
       <c r="H24" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61538461538461542</v>
+        <v>0.77319330909986494</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1990,15 +1997,15 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70061592883415724</v>
+        <v>0.35750860626682435</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0123185766831444</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5010265480569287</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="3"/>
@@ -2016,15 +2023,15 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9560207958790228E-2</v>
+        <v>0.7526436229151654</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7.0528724583033071</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.58773937152527556</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="3"/>
@@ -2041,6 +2048,198 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <f>ROUND((36-B3)/3.2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3-1</f>
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C19" si="0">ROUND((36-B4)/3.2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ref="B5:B17" si="1">B4-1</f>
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>B15-1</f>
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>B17-1</f>
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>B18-1</f>
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F12"/>
   <sheetViews>
@@ -2263,7 +2462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F32"/>
   <sheetViews>
@@ -2656,7 +2855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
@@ -2752,11 +2951,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#35 #93 #10 #25 #87 #74 #88 #83 #94 #95 #81 #92 #80 #89 #91 #86 #60 #43 #98 #46 #64 #65 #58 #85 #11
</commit_message>
<xml_diff>
--- a/documentation/charts.xlsx
+++ b/documentation/charts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoS\Documents\Arma 3\missions\SATGv2.Chernarus_winter\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoS\Documents\Arma 3\missions\SATGv2.git\branches\develop\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WORLD TEMP" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>ОБЛАЧНОСТЬ</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>IMAGE</t>
+  </si>
+  <si>
+    <t>INTERCEPT</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H26"/>
+  <dimension ref="B2:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1402,7 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1418,22 +1421,25 @@
       <c r="H2" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3">
         <f ca="1">RAND()</f>
-        <v>0.70495548776819184</v>
+        <v>0.67283878614660753</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">MAX((C3-0.4)*20,0)</f>
-        <v>6.0991097553638358</v>
+        <v>5.4567757229321501</v>
       </c>
       <c r="F3" s="3">
         <f ca="1">E3/12</f>
-        <v>0.50825914628031965</v>
+        <v>0.45473131024434582</v>
       </c>
       <c r="G3" s="3">
         <f>ABS(14-B3)/13</f>
@@ -1443,15 +1449,19 @@
         <f ca="1">MAX(F3,G3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="5">
+        <f ca="1">(E3/12)*7+7</f>
+        <v>10.18311917171042</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C26" ca="1" si="0">RAND()</f>
-        <v>0.29920265833098536</v>
+        <v>0.31565878571823458</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E26" ca="1" si="1">MAX((C4-0.4)*20,0)</f>
@@ -1469,23 +1479,27 @@
         <f t="shared" ref="H4:H26" ca="1" si="4">MAX(F4,G4)</f>
         <v>0.92307692307692313</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I26" ca="1" si="5">(E4/12)*7+7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
-        <f t="shared" ref="B5:B26" si="5">B4+1</f>
+        <f t="shared" ref="B5:B26" si="6">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7473401375907875E-2</v>
+        <v>0.96033875868348217</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>11.206775173669643</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.93389793113913688</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="3"/>
@@ -1493,25 +1507,29 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.84615384615384615</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.93389793113913688</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>13.537285517973958</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97892311775729079</v>
+        <v>0.75720014584132378</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11.578462355145815</v>
+        <v>7.1440029168264747</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96487186292881788</v>
+        <v>0.59533357640220619</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="3"/>
@@ -1519,25 +1537,29 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.96487186292881788</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>11.167335034815444</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53602725968137954</v>
+        <v>6.5699594590201027E-2</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7205451936275904</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22671209946896587</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="3"/>
@@ -1547,23 +1569,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.69230769230769229</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9046661323971007</v>
+        <v>0.38999240793102352</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.093322647942014</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8411102206618345</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="3"/>
@@ -1571,25 +1597,29 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.8411102206618345</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86568084261055411</v>
+        <v>0.18469950652638956</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3136168522110818</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77613473768425678</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="3"/>
@@ -1597,25 +1627,29 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.77613473768425678</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69099063117876469</v>
+        <v>6.5141167810849332E-2</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8198126235752934</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.48498438529794113</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="3"/>
@@ -1623,25 +1657,29 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.48498438529794113</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49735511489268458</v>
+        <v>0.50036708597129009</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9471022978536912</v>
+        <v>2.0073417194258014</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16225852482114092</v>
+        <v>0.16727847661881678</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="3"/>
@@ -1651,23 +1689,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.38461538461538464</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="5">
+        <f ca="1">(E11/12)*7+7</f>
+        <v>8.1709493363317165</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86026390224790439</v>
+        <v>0.71301382134059399</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2052780449580869</v>
+        <v>6.2602764268118793</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76710650374650724</v>
+        <v>0.52168970223432332</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="3"/>
@@ -1675,25 +1717,29 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.76710650374650724</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.52168970223432332</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.651827915640263</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68477968438556835</v>
+        <v>0.30304094244582513</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6955936877113666</v>
+        <v>0</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47463280730928054</v>
+        <v>0</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="3"/>
@@ -1701,17 +1747,21 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.47463280730928054</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25031236403669199</v>
+        <v>0.18013337253084949</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -1729,23 +1779,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.15384615384615385</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16807731447506447</v>
+        <v>0.5159333166180945</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.3186663323618895</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.19322219436349078</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="3"/>
@@ -1753,25 +1807,29 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.19322219436349078</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>8.3525553605444358</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52521571772110043</v>
+        <v>0.10251507588965769</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5043143544220081</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.20869286286850067</v>
+        <v>0</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="3"/>
@@ -1779,25 +1837,29 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.20869286286850067</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38874889248844335</v>
+        <v>0.79056201879830279</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7.8112403759660554</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.65093669799717124</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="3"/>
@@ -1805,25 +1867,29 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.65093669799717124</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>11.5565568859802</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C18" s="3">
         <f ca="1">RAND()</f>
-        <v>0.51242450550358554</v>
+        <v>0.35376068554859796</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2484901100717103</v>
+        <v>0</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.18737417583930918</v>
+        <v>0</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="3"/>
@@ -1831,25 +1897,29 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.18737417583930918</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15683169422185195</v>
+        <v>0.60418147325570815</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4.0836294651141625</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.34030245542618021</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="3"/>
@@ -1857,25 +1927,29 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.23076923076923078</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.34030245542618021</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>9.3821171879832619</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27567675512286371</v>
+        <v>0.42730880061977283</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>0.54617601239545621</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4.5514667699621349E-2</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="3"/>
@@ -1885,23 +1959,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.30769230769230771</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.3186026738973498</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5787651167845328</v>
+        <v>0.81922201795486205</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5753023356906555</v>
+        <v>8.3844403590972405</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29794186130755462</v>
+        <v>0.69870336325810334</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="3"/>
@@ -1909,25 +1987,29 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.38461538461538464</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.69870336325810334</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>11.890923542806723</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92410924680525419</v>
+        <v>0.24248415458367356</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.482184936105083</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87351541134209032</v>
+        <v>0</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="3"/>
@@ -1935,25 +2017,29 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.87351541134209032</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29303778344106191</v>
+        <v>0.52580761535013898</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.5161523070027791</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>0.20967935891689826</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="3"/>
@@ -1963,23 +2049,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.53846153846153844</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>8.4677555124182877</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86391598545991899</v>
+        <v>0.68711823989639109</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2783197091983798</v>
+        <v>5.7423647979278218</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77319330909986494</v>
+        <v>0.47853039982731849</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="3"/>
@@ -1987,17 +2077,21 @@
       </c>
       <c r="H24" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.77319330909986494</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.349712798791229</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35750860626682435</v>
+        <v>0.30584635614364708</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" ca="1" si="1"/>
@@ -2015,23 +2109,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0.69230769230769229</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7526436229151654</v>
+        <v>0.42123406414466547</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0528724583033071</v>
+        <v>0.42468128289330886</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>0.58773937152527556</v>
+        <v>3.5390106907775741E-2</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="3"/>
@@ -2040,6 +2138,10 @@
       <c r="H26" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>0.76923076923076927</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.2477307483544298</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C19"/>
     </sheetView>
   </sheetViews>
@@ -2955,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>